<commit_message>
addded stats, did tables and fig, ned bias and interaction
</commit_message>
<xml_diff>
--- a/tabs.xlsx
+++ b/tabs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="19920" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19920" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>household</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Surface water used for drinking</t>
+  </si>
+  <si>
+    <t>Adjusted RR</t>
+  </si>
+  <si>
+    <t>* adjusted for age</t>
+  </si>
+  <si>
+    <t>do not</t>
   </si>
 </sst>
 </file>
@@ -170,8 +179,8 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -181,7 +190,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1209675" y="1323976"/>
-          <a:ext cx="1238250" cy="704850"/>
+          <a:ext cx="1238250" cy="447674"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -216,9 +225,17 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Exposure to Cryptosporidium parvum oocysts</a:t>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>produce own food</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -234,8 +251,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -245,7 +262,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3952875" y="1304926"/>
-          <a:ext cx="1238250" cy="704850"/>
+          <a:ext cx="1238250" cy="476249"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -357,80 +374,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>561975</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="352425" y="314325"/>
-          <a:ext cx="685800" cy="561974"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>produce own food</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -439,7 +391,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="219074" y="2400300"/>
+          <a:off x="561975" y="314325"/>
           <a:ext cx="1457325" cy="647700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -490,79 +442,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>338136</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>123827</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="6" idx="0"/>
-          <a:endCxn id="2" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="1202531" y="1774032"/>
-          <a:ext cx="371474" cy="881063"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>71439</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="10" name="Straight Arrow Connector 9"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="5" idx="3"/>
+          <a:stCxn id="6" idx="2"/>
           <a:endCxn id="2" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1038225" y="595312"/>
-          <a:ext cx="790575" cy="728664"/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1378744" y="873919"/>
+          <a:ext cx="361951" cy="538162"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -655,12 +557,12 @@
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="3" idx="0"/>
-          <a:endCxn id="4" idx="2"/>
+          <a:stCxn id="4" idx="2"/>
+          <a:endCxn id="3" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipV="1">
+        <a:xfrm rot="16200000" flipH="1">
           <a:off x="3576637" y="309563"/>
           <a:ext cx="428626" cy="1562100"/>
         </a:xfrm>
@@ -668,6 +570,57 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23813</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2447925" y="1543051"/>
+          <a:ext cx="1504950" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:prstDash val="dash"/>
           <a:tailEnd type="arrow"/>
         </a:ln>
       </xdr:spPr>
@@ -978,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,19 +1041,19 @@
         <v>4</v>
       </c>
       <c r="D14">
-        <v>1303</v>
+        <v>845</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" ref="E14:E16" si="0">D14/$D$8</f>
-        <v>0.78636089318044655</v>
+        <v>0.50995775497887752</v>
       </c>
       <c r="F14">
         <f t="shared" ref="F14:F16" si="1">$D$8-D14</f>
-        <v>354</v>
+        <v>812</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ref="G14:G16" si="2">F14/$D$8</f>
-        <v>0.21363910681955342</v>
+        <v>0.49004224502112254</v>
       </c>
     </row>
     <row r="15" spans="2:7">
@@ -1357,12 +1310,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7">
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <f>678</f>
+        <v>678</v>
+      </c>
+      <c r="E4">
+        <f>E6-E5</f>
+        <v>133</v>
+      </c>
+      <c r="F4" s="1">
+        <f>D4/E4</f>
+        <v>5.0977443609022552</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <f>D6-D4</f>
+        <v>364</v>
+      </c>
+      <c r="E5">
+        <v>482</v>
+      </c>
+      <c r="F5" s="1">
+        <f>D5/E5</f>
+        <v>0.75518672199170123</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="D6">
+        <v>1042</v>
+      </c>
+      <c r="E6">
+        <v>615</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1371,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>